<commit_message>
Update leaderboard and data
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FA6134-E047-4DFF-983B-7378D37621F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0D666F-5DEF-488E-B8B4-555B693974F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Customer Name</t>
   </si>
@@ -80,6 +80,18 @@
   </si>
   <si>
     <t>013</t>
+  </si>
+  <si>
+    <t>Isaac's Pub</t>
+  </si>
+  <si>
+    <t>Frisch, Isaac</t>
+  </si>
+  <si>
+    <t>State Street</t>
+  </si>
+  <si>
+    <t>Reciprical Show</t>
   </si>
 </sst>
 </file>
@@ -441,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -579,16 +591,46 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45848</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45848</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3">
+        <v>45848</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Major UI improvements: Added overview section, streamlined leaderboard, tabbed customer views, Futura font, and file-based timestamps
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\OneDrive - Van Paper Company\Python_Projects\Sales_Leaderboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AE782D2-B5C7-4CEA-81E6-66EC98678179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B0D5CFE-F652-4F64-96A3-F62440E8F914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
     <t>Bearpath- Paper Products</t>
   </si>
   <si>
-    <t>Palmar</t>
+    <t>PALMAR MEXICAN RESTAURANT</t>
   </si>
   <si>
     <t>VALLEY OFFICE PARK</t>
@@ -206,7 +206,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -535,7 +535,7 @@
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -562,9 +562,8 @@
       <c r="D2" s="2">
         <v>45869</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -575,11 +574,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <v>45883</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45868</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -592,9 +590,8 @@
       <c r="D4" s="2">
         <v>45883</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -607,9 +604,8 @@
       <c r="D5" s="2">
         <v>45884</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -622,9 +618,8 @@
       <c r="D6" s="2">
         <v>45883</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -635,9 +630,8 @@
         <v>14</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -648,9 +642,8 @@
         <v>14</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -661,9 +654,8 @@
         <v>9</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -674,11 +666,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="2">
-        <v>45888</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45874</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -689,11 +680,10 @@
         <v>21</v>
       </c>
       <c r="D11" s="2">
-        <v>45880</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45849</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -704,11 +694,10 @@
         <v>21</v>
       </c>
       <c r="D12" s="2">
-        <v>45881</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45845</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -719,9 +708,8 @@
         <v>9</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -732,9 +720,8 @@
         <v>6</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -747,9 +734,8 @@
       <c r="D15" s="2">
         <v>45855</v>
       </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -760,9 +746,8 @@
         <v>9</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -775,9 +760,8 @@
       <c r="D17" s="2">
         <v>45873</v>
       </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -790,9 +774,8 @@
       <c r="D18" s="2">
         <v>45883</v>
       </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -803,9 +786,8 @@
         <v>6</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -816,9 +798,8 @@
         <v>9</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -829,9 +810,8 @@
         <v>14</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -844,9 +824,8 @@
       <c r="D22" s="2">
         <v>45881</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -859,9 +838,8 @@
       <c r="D23" s="2">
         <v>45883</v>
       </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -872,9 +850,8 @@
         <v>6</v>
       </c>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -885,9 +862,8 @@
         <v>31</v>
       </c>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -898,9 +874,8 @@
         <v>9</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -908,12 +883,11 @@
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -926,9 +900,8 @@
       <c r="D28" s="2">
         <v>45847</v>
       </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
@@ -941,9 +914,8 @@
       <c r="D29" s="2">
         <v>45888</v>
       </c>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -954,9 +926,8 @@
         <v>21</v>
       </c>
       <c r="D30" s="2">
-        <v>45889</v>
-      </c>
-      <c r="E30" s="3"/>
+        <v>45848</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix data processing logic and leaderboard display - resolve Excel column mapping and rule violation detection
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\OneDrive - Van Paper Company\Python_Projects\Sales_Leaderboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B0D5CFE-F652-4F64-96A3-F62440E8F914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BE98D6D-F3AE-425A-8E07-5050C4441EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>Customer Name</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Last Invoice Date</t>
   </si>
   <si>
+    <t>Customer Number</t>
+  </si>
+  <si>
     <t>MILL CITY SOUND</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t>013</t>
   </si>
   <si>
+    <t>0008143</t>
+  </si>
+  <si>
     <t>ROYAL GOLF CLUB</t>
   </si>
   <si>
@@ -52,33 +58,57 @@
     <t>015</t>
   </si>
   <si>
+    <t>0008176</t>
+  </si>
+  <si>
     <t>PAUL'S WINE &amp; SPIRITS</t>
   </si>
   <si>
     <t>Dack, Suzanne</t>
   </si>
   <si>
+    <t>0008179</t>
+  </si>
+  <si>
     <t>ADAIR LIQUORS</t>
   </si>
   <si>
+    <t>0008180</t>
+  </si>
+  <si>
+    <t>0008181</t>
+  </si>
+  <si>
     <t>Cassini's Pizza</t>
   </si>
   <si>
     <t>040</t>
   </si>
   <si>
+    <t>0008189</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cassini's Pizza </t>
   </si>
   <si>
+    <t>0008191</t>
+  </si>
+  <si>
     <t>Jimmy's Food &amp; Drink</t>
   </si>
   <si>
+    <t>0008193</t>
+  </si>
+  <si>
     <t>IVY LEAGUE PLACE</t>
   </si>
   <si>
     <t>Steiner, Owen A</t>
   </si>
   <si>
+    <t>0008196</t>
+  </si>
+  <si>
     <t>CASA MAYA #1</t>
   </si>
   <si>
@@ -88,79 +118,139 @@
     <t>023</t>
   </si>
   <si>
+    <t>0008198</t>
+  </si>
+  <si>
     <t>CASA MAYA GRILL #2</t>
   </si>
   <si>
+    <t>0008199</t>
+  </si>
+  <si>
     <t>Bierstube</t>
   </si>
   <si>
+    <t>0008204</t>
+  </si>
+  <si>
     <t>SUNDAYS CA PHE</t>
   </si>
   <si>
     <t>House Account</t>
   </si>
   <si>
+    <t>0008209</t>
+  </si>
+  <si>
     <t>WHITE FRONT INC</t>
   </si>
   <si>
     <t>Monroe, Michael D</t>
   </si>
   <si>
+    <t>0008213</t>
+  </si>
+  <si>
     <t>Hoagie's Family Restaurant</t>
   </si>
   <si>
+    <t>0008217</t>
+  </si>
+  <si>
     <t>ST PAUL INDOOR FARMER'S MARKET</t>
   </si>
   <si>
+    <t>0008226</t>
+  </si>
+  <si>
     <t>BARISTA COFFEE BAR</t>
   </si>
   <si>
     <t>030</t>
   </si>
   <si>
+    <t>0008227</t>
+  </si>
+  <si>
     <t>THE PERFECT PICKLE</t>
   </si>
   <si>
+    <t>0008229</t>
+  </si>
+  <si>
     <t>Stockyards</t>
   </si>
   <si>
+    <t>0008231</t>
+  </si>
+  <si>
     <t>CRYSTAL LAKE GOLF CLUB</t>
   </si>
   <si>
+    <t>0008237</t>
+  </si>
+  <si>
     <t>COURY CARTAGE</t>
   </si>
   <si>
     <t>Bloch, Lea L</t>
   </si>
   <si>
+    <t>0008239</t>
+  </si>
+  <si>
     <t>BEAR PAW PAPERWORKS</t>
   </si>
   <si>
+    <t>0008241</t>
+  </si>
+  <si>
     <t>Mr Mustacheo</t>
   </si>
   <si>
+    <t>0008242</t>
+  </si>
+  <si>
     <t>BEE SWEET LLC</t>
   </si>
   <si>
     <t>Ballman, John W</t>
   </si>
   <si>
+    <t>0008246</t>
+  </si>
+  <si>
     <t>Bearpath- Paper Products</t>
   </si>
   <si>
+    <t>0008247</t>
+  </si>
+  <si>
     <t>PALMAR MEXICAN RESTAURANT</t>
   </si>
   <si>
+    <t>0008249</t>
+  </si>
+  <si>
     <t>VALLEY OFFICE PARK</t>
   </si>
   <si>
     <t>003</t>
   </si>
   <si>
+    <t>0005754</t>
+  </si>
+  <si>
     <t>HOME FIRES PIZZA &amp; PROVISIONS</t>
   </si>
   <si>
+    <t>0007240</t>
+  </si>
+  <si>
     <t>BAKER AND LOVER INC</t>
+  </si>
+  <si>
+    <t>0007391</t>
   </si>
 </sst>
 </file>
@@ -522,7 +612,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -531,11 +621,12 @@
     <col min="1" max="1" width="51.5703125" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,385 +639,475 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>45869</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <v>45868</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="2">
         <v>45883</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D5" s="2">
         <v>45884</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D6" s="2">
         <v>45883</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D10" s="2">
         <v>45874</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2">
         <v>45849</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2">
         <v>45845</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2">
         <v>45855</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D17" s="2">
         <v>45873</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2">
         <v>45883</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22" s="2">
         <v>45881</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D23" s="2">
         <v>45883</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2">
         <v>45847</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D29" s="2">
         <v>45888</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D30" s="2">
         <v>45848</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Outlook email automation for Van Paper reports - auto-downloads and updates leaderboard
</commit_message>
<xml_diff>
--- a/leaderboard.xlsx
+++ b/leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\OneDrive - Van Paper Company\Python_Projects\Sales_Leaderboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BE98D6D-F3AE-425A-8E07-5050C4441EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{98C21B0C-D353-4429-93BB-F5DE04111B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>Customer Name</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>0008249</t>
+  </si>
+  <si>
+    <t>Galvan Foods</t>
+  </si>
+  <si>
+    <t>0008254</t>
   </si>
   <si>
     <t>VALLEY OFFICE PARK</t>
@@ -612,9 +618,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1064,30 +1072,28 @@
         <v>70</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D28" s="2">
-        <v>45847</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="D29" s="2">
-        <v>45888</v>
+        <v>45847</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>74</v>
@@ -1101,13 +1107,30 @@
         <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D30" s="2">
-        <v>45848</v>
+        <v>45888</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="2">
+        <v>45848</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>